<commit_message>
43, 63 added; 40 changed
</commit_message>
<xml_diff>
--- a/Задания по SQL.xlsx
+++ b/Задания по SQL.xlsx
@@ -718,17 +718,6 @@
 group by maker</t>
   </si>
   <si>
-    <t>with v0 as (
-select maker, type, count(*) as models
-            from product
-            group by maker, type)
-select maker,type
-from v0
-group by maker
-having count(*) = 1
-and sum(models)&gt;1</t>
-  </si>
-  <si>
     <t>WITH v0 AS (
   SELECT
     ship,
@@ -1513,10 +1502,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Неверное число записей (меньше на 3)
-</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -1642,6 +1627,32 @@
 FROM v0
 WHERE sunk &gt; 0
   AND c &gt;=3</t>
+  </si>
+  <si>
+    <t>WITH v0 AS (
+  SELECT
+    maker,
+    type,
+    COUNT(1) AS c
+  FROM product
+  GROUP BY maker, type
+),v1 AS (
+  SELECT
+    maker
+  FROM v0
+  GROUP BY maker
+  HAVING COUNT(1) = 1
+)
+SELECT
+  b.maker, b.type
+FROM v1 a
+  LEFT JOIN v0 b
+    ON a.maker = b.maker
+WHERE c &gt; 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">не прошел тест на проверочной базе
+</t>
   </si>
 </sst>
 </file>
@@ -1794,11 +1805,19 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -2131,7 +2150,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,13 +2180,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2247,7 +2266,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>29</v>
@@ -2325,7 +2344,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
@@ -2341,7 +2360,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>15</v>
@@ -2357,7 +2376,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>67</v>
@@ -2373,7 +2392,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>13</v>
@@ -2389,7 +2408,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
@@ -2405,7 +2424,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>10</v>
@@ -2421,7 +2440,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
@@ -2437,7 +2456,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
@@ -2453,7 +2472,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>31</v>
@@ -2485,7 +2504,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>66</v>
@@ -2494,7 +2513,7 @@
         <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F26" s="13"/>
     </row>
@@ -2503,16 +2522,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F27" s="11"/>
     </row>
@@ -2521,7 +2540,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>38</v>
@@ -2548,7 +2567,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2564,12 +2583,12 @@
       <c r="E30" s="1"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>64</v>
@@ -2613,7 +2632,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>50</v>
@@ -2629,7 +2648,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>63</v>
@@ -2645,7 +2664,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>59</v>
@@ -2656,7 +2675,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="16"/>
     </row>
-    <row r="37" spans="1:8" ht="78.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2670,7 +2689,7 @@
         <v>54</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F37" s="12"/>
     </row>
@@ -2705,7 +2724,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2713,36 +2732,36 @@
         <v>69</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F40" s="13"/>
     </row>
-    <row r="41" spans="1:8" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F41" s="12"/>
+        <v>170</v>
+      </c>
+      <c r="F41" s="11"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="223.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2759,7 +2778,7 @@
         <v>73</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F42" s="13"/>
     </row>
@@ -2787,13 +2806,13 @@
         <v>77</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F44" s="12"/>
     </row>
@@ -2802,16 +2821,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F45" s="13"/>
     </row>
@@ -2820,13 +2839,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="11"/>
@@ -2836,16 +2855,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F47" s="13"/>
     </row>
@@ -2854,16 +2873,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F48" s="11"/>
     </row>
@@ -2872,13 +2891,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="11"/>
@@ -2888,13 +2907,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="11"/>
@@ -2904,10 +2923,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>4</v>
@@ -2920,13 +2939,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="F52" s="14"/>
     </row>
@@ -2935,13 +2954,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E53" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F53" s="13"/>
     </row>
@@ -2950,16 +2969,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F54" s="13"/>
     </row>
@@ -2968,16 +2987,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F55" s="13"/>
     </row>
@@ -2986,13 +3005,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="11"/>
@@ -3002,10 +3021,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="11"/>
@@ -3015,13 +3034,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F58" s="13"/>
     </row>
@@ -3030,13 +3049,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F59" s="11"/>
     </row>
@@ -3045,25 +3064,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F60" s="13"/>
     </row>
-    <row r="61" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="15"/>
@@ -3082,30 +3101,30 @@
       <c r="C63" s="6"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" s="6" t="s">
         <v>119</v>
       </c>
+      <c r="C64" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="E64" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F64" s="12"/>
-    </row>
-    <row r="65" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="F64" s="13"/>
+    </row>
+    <row r="65" spans="1:8" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="11"/>
@@ -3134,18 +3153,18 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="11"/>
@@ -3155,10 +3174,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="11"/>
@@ -3168,16 +3187,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C72" s="6" t="s">
-        <v>152</v>
-      </c>
       <c r="D72" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="F72" s="16"/>
     </row>
@@ -3186,13 +3205,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="F73" s="13"/>
     </row>
@@ -3201,18 +3220,18 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="11"/>
       <c r="H74" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="240" hidden="1" x14ac:dyDescent="0.25">
@@ -3220,10 +3239,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="11"/>
@@ -3240,59 +3259,41 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="405" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>56</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="2"/>
     </row>
   </sheetData>
-  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:G80">
-    <filterColumn colId="2">
-      <filters>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <x14:filter val="-- вывести список классов кораблей которые участвовали в битвах с четным числом_x000a_-- outcomes(ship,battle), battles(name,date)_x000a_-- /2==0_x000a_WITH potential_ships AS (_x000a_  SELECT_x000a_    name,_x000a_    class_x000a_  FROM Ships_x000a_  UNION_x000a_  SELECT_x000a_    class,_x000a_    class_x000a_  FROM Classes_x000a_)_x000a_SELECT_x000a_  class,_x000a_  SUM(_x000a_    CASE WHEN b.date % 2 = 0 THEN 1_x000a_         ELSE 0 END_x000a_    )_x000a_FROM potential_ships p_x000a_  LEFT JOIN Outcomes o_x000a_    ON o.ship = p.name_x000a_  LEFT JOIN Battles b_x000a_    ON b.name = o.battle_x000a_GROUP BY class;"/>
-            <x14:filter val="Select coalesce(a.point, b.point), coalesce(a.date, b.date), inc, out_x000a_from income_o a_x000a_full outer join outcome_o b on a.point=b.point and a.date=b.date_x000a__x000a_или_x000a__x000a_Select case when (a.point is null) then b.point else a.point end as point,_x000a_case when (a.date is null) then b.date else a.date end as date, inc as income, out as outcome_x000a_from income_o a full outer join outcome_o b on a.point=b.point and a.date=b.date_x000a_"/>
-            <x14:filter val="select coalesce(a.point, b.point), coalesce(a.date, b.date), sum(out), sum(inc)_x000a_from income a _x000a_full outer join outcome b on a.point=b.point and a.date=b.date_x000a_group by coalesce(a.point, b.point), coalesce(a.date, b.date)_x000a_Where a.date&lt;'20010415' and b.date&lt;'20010415'_x000a_"/>
-            <x14:filter val="Select coalesce(a.point, b.point), coalesce(a.date, b.date), sum(out), sum(inc)_x000a_from income a_x000a_full outer join outcome b on a.code=b.code and a.point=b.point and a.date=b.date_x000a_group by coalesce(a.point, b.point), coalesce(a.date, b.date)_x000a__x000a_или_x000a__x000a_Select case when (a.point is null) then b.point else a.point end as point, case when (a.date is null) then b.date else a.date end as date, sum(out), sum(inc)_x000a_from income a_x000a_full outer join outcome b on a.code=b.code and a.point=b.point and a.date=b.date_x000a_group by case when (a.point is null) then b.point else a.point end, case when (a.date is null) then b.date else a.date end"/>
-            <x14:filter val="Select count(a.trip_no) as count, date_x000a_from trip a_x000a_left join Pass_in_trip b on a.trip_no=b.trip_no_x000a_where town_from='Rostov'_x000a_group by date_x000a_"/>
-            <x14:filter val="select name_x000a_from battles_x000a_where year(date) not in (select year(launched) from ships) and date is not null_x000a_"/>
-            <x14:filter val="with income_0 as (_x000a_select point, date, sum(inc) as dayinc_x000a_from income_x000a_group by point, date_x000a_), outcome_0 as (_x000a_select distinct point, date, sum(out) as dayout_x000a_from outcome_x000a_group by point, date_x000a_)_x000a_select_x000a_coalesce(a.point, b.point) as point, coalesce(a.date, b.date) as date,_x000a_case when (a.dayinc is null) then 'out' _x000a_when (b.dayout is null) then 'inc' end as operation,_x000a_case when (a.dayinc is null) then b.dayout _x000a_when (b.dayout is null) then a.dayinc_x000a_end as money_sum_x000a_from income_0 a full outer join outcome_0 b on a.point=b.point and a.date=b.date_x000a_where (a.point is null or b.point is null)"/>
-            <x14:filter val="WITH incomes AS (_x000a_  SELECT_x000a_    point,_x000a_    date,_x000a_    SUM(inc) AS dayinc_x000a_  FROM Income_x000a_  WHERE inc IS NOT NULL_x000a_  GROUP BY point, date_x000a_),outcomes AS (_x000a_  SELECT_x000a_    point,_x000a_    date,_x000a_    SUM(out) AS dayout_x000a_  FROM Outcome_x000a_  WHERE out IS NOT NULL_x000a_  GROUP BY point, date_x000a_),totals AS (_x000a_  SELECT_x000a_    COALESCE(a.point, b.point) AS point,_x000a_    COALESCE(a.date, b.date) AS date,_x000a_    COALESCE(a.dayinc, 0) - COALESCE(b.dayout, 0) AS total_x000a_  FROM incomes a_x000a_    full OUTER JOIN outcomes b_x000a_      ON a.point = b.point AND a.date = b.date_x000a_)_x000a_SELECT_x000a_  point,_x000a_--    DATETIME(ROUND(date / 1000), 'unixepoch')_x000a_ convert(varchar(10),    date, 103)_x000a_  AS day,_x000a_--total,_x000a_--lag(total) over(partition by point order by date) as previous_total,_x000a_--lead(total) over(partition by point order by date) as next_total,_x000a_sum(total) over (partition by point order by date) as total_rolling_x000a__x000a_FROM totals_x000a_order by point, date_x000a_"/>
-            <x14:filter val="WITH v0 AS (_x000a_  SELECT_x000a_    ship,_x000a_    date,_x000a_    result_x000a_  FROM Outcomes a_x000a_    LEFT JOIN Battles b_x000a_      ON a.battle = b.name_x000a_)_x000a_SELECT *_x000a_ --DISTINCT a.ship_x000a_FROM v0 a_x000a_  LEFT JOIN v0 b_x000a_    ON a.ship = b.ship_x000a_AND a.date &lt; b.date_x000a_WHERE a.result in ('OK' ,'damaged')_x000a_  AND b.result in ('OK',null)"/>
-          </mc:Choice>
-          <mc:Fallback>
-            <filter val="Select count(a.trip_no) as count, date_x000a_from trip a_x000a_left join Pass_in_trip b on a.trip_no=b.trip_no_x000a_where town_from='Rostov'_x000a_group by date_x000a_"/>
-            <filter val="select name_x000a_from battles_x000a_where year(date) not in (select year(launched) from ships) and date is not null_x000a_"/>
-          </mc:Fallback>
-        </mc:AlternateContent>
-      </filters>
+  <autoFilter ref="A1:G80">
+    <filterColumn colId="5">
+      <colorFilter dxfId="0"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
36 in Ships added
</commit_message>
<xml_diff>
--- a/Задания по SQL.xlsx
+++ b/Задания по SQL.xlsx
@@ -312,14 +312,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Использование в запросе нескольких источников записей</t>
-  </si>
-  <si>
-    <t>Select ship
-from outcomes 
-union
-select name
-from ships
-where name=class</t>
   </si>
   <si>
     <t>Перечислите названия головных кораблей, имеющихся в базе данных (учесть корабли в Outcomes).</t>
@@ -1137,36 +1129,6 @@
     ON v0.maker = v1.maker</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">select name
-from battles
-where </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>year(date)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> not in (select year(launched) from ships) and date is not null
-</t>
-    </r>
-  </si>
-  <si>
     <t>Вывести все классы кораблей России (Russia). Если в базе данных нет классов кораблей России, вывести классы для всех имеющихся в БД стран.
 Вывод: страна, класс</t>
   </si>
@@ -1653,6 +1615,21 @@
   <si>
     <t xml:space="preserve">не прошел тест на проверочной базе
 </t>
+  </si>
+  <si>
+    <t>select name
+from battles
+where year(date) not in (select launched from ships)</t>
+  </si>
+  <si>
+    <t>select ship
+from Outcomes
+left join Classes on ship=class
+where ship=class
+union
+select name
+from Ships
+where name=class</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1678,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1717,12 +1694,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1751,7 +1722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1789,16 +1760,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2145,12 +2113,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,16 +2147,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2197,7 +2164,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2205,7 +2172,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2213,7 +2180,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2221,7 +2188,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2229,7 +2196,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2237,7 +2204,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2245,7 +2212,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2253,7 +2220,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2261,12 +2228,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>29</v>
@@ -2275,7 +2242,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2291,7 +2258,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2307,7 +2274,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2323,7 +2290,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2339,12 +2306,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
@@ -2355,12 +2322,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="75.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>15</v>
@@ -2371,15 +2338,15 @@
       <c r="E17" s="1"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>30</v>
@@ -2387,12 +2354,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>13</v>
@@ -2403,12 +2370,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
@@ -2419,12 +2386,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>10</v>
@@ -2435,12 +2402,12 @@
       <c r="E21" s="1"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>9</v>
@@ -2451,12 +2418,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
@@ -2467,12 +2434,12 @@
       <c r="E23" s="1"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:6" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>31</v>
@@ -2483,7 +2450,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:6" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2499,48 +2466,48 @@
       <c r="E25" s="1"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:6" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:6" ht="255" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>38</v>
@@ -2551,7 +2518,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2559,7 +2526,7 @@
         <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>40</v>
@@ -2567,7 +2534,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="1:6" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2583,15 +2550,15 @@
       <c r="E30" s="1"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="1:6" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>43</v>
@@ -2599,7 +2566,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2612,7 +2579,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:8" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2623,16 +2590,16 @@
         <v>48</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>50</v>
@@ -2643,15 +2610,15 @@
       <c r="E34" s="1"/>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>51</v>
@@ -2659,141 +2626,141 @@
       <c r="E35" s="1"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="16"/>
+      <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="1:8" ht="210" hidden="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="1:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F40" s="13"/>
-    </row>
-    <row r="41" spans="1:8" ht="300" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="223.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F42" s="13"/>
-    </row>
-    <row r="43" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="11"/>
@@ -2802,131 +2769,131 @@
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>170</v>
+      <c r="E44" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:8" ht="315" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F45" s="13"/>
-    </row>
-    <row r="46" spans="1:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="11"/>
     </row>
-    <row r="47" spans="1:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F47" s="13"/>
-    </row>
-    <row r="48" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F48" s="11"/>
     </row>
-    <row r="49" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="11"/>
     </row>
-    <row r="50" spans="1:6" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="11"/>
     </row>
-    <row r="51" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>4</v>
@@ -2934,167 +2901,167 @@
       <c r="E51" s="1"/>
       <c r="F51" s="11"/>
     </row>
-    <row r="52" spans="1:6" s="9" customFormat="1" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="9" customFormat="1" ht="405" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52" s="14"/>
-    </row>
-    <row r="53" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="E53" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F53" s="13"/>
-    </row>
-    <row r="54" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F54" s="13"/>
-    </row>
-    <row r="55" spans="1:6" ht="330" hidden="1" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" spans="1:6" ht="330" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F55" s="13"/>
-    </row>
-    <row r="56" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="11"/>
     </row>
-    <row r="57" spans="1:6" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="11"/>
     </row>
-    <row r="58" spans="1:6" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F58" s="13"/>
-    </row>
-    <row r="59" spans="1:6" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="F58" s="12"/>
+    </row>
+    <row r="59" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F59" s="11"/>
     </row>
-    <row r="60" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F60" s="13"/>
-    </row>
-    <row r="61" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="E61" s="1"/>
-      <c r="F61" s="15"/>
-    </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="C62" s="6"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3105,197 +3072,193 @@
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>119</v>
+      <c r="B64" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F64" s="13"/>
-    </row>
-    <row r="65" spans="1:8" ht="285" hidden="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="11"/>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="11"/>
     </row>
-    <row r="71" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="11"/>
     </row>
-    <row r="72" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F72" s="16"/>
-    </row>
-    <row r="73" spans="1:8" ht="255" hidden="1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="F72" s="15"/>
+    </row>
+    <row r="73" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F73" s="13"/>
-    </row>
-    <row r="74" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F73" s="12"/>
+    </row>
+    <row r="74" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="11"/>
       <c r="H74" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="240" hidden="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="11"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="405" hidden="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="405" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>56</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F80" s="15" t="s">
-        <v>178</v>
+        <v>162</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G80">
-    <filterColumn colId="5">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G80"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
75, 76, 89 were added, but they are not finished
</commit_message>
<xml_diff>
--- a/Задания по SQL.xlsx
+++ b/Задания по SQL.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$G$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$G$85</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="224">
   <si>
     <t>Запрос:</t>
   </si>
@@ -1796,45 +1796,78 @@
   <si>
     <t>with v0 as (
 Select name,
-case when (numGuns = 8 and bore = 15 and displacement = 32000 and type = 'bb')
-then 1
-when (numGuns = 8 and bore = 15 and displacement = 32000 and launched = 1915)
-then 1
-when (numGuns = 8 and bore = 15 and displacement = 32000 and a.class='Kongo')
-then 1
-when (numGuns = 8 and bore = 15 and displacement = 32000 and country='USA')
-then 1
-when (bore = 15 and displacement = 32000 and type = 'bb' and launched = 1915)
-then 1
-when (bore = 15 and displacement = 32000 and type = 'bb' and a.class='Kongo')
-then 1
-when (bore = 15 and displacement = 32000 and type = 'bb' and country='USA')
-then 1
-when (displacement = 32000 and type = 'bb' and launched = 1915 and a.class='Kongo')
-then 1
-when (displacement = 32000 and type = 'bb' and launched = 1915 and country='USA')
-then 1
-when (type = 'bb' and launched = 1915 and a.class='Kongo' and country='USA')
-then 1
-when (numGuns = 8 and displacement = 32000 and launched = 1915 and a.class='Kongo')
-then 1
-when (numGuns = 8 and displacement = 32000 and launched = 1915 and country='USA')
-then 1
-when (numGuns = 8 and type = 'bb' and launched = 1915 and a.class='Kongo')
-then 1
-when (numGuns = 8 and type = 'bb' and launched = 1915 and country='USA')
-then 1
-when (bore = 15 and type = 'bb' and launched = 1915 and a.class='Kongo')
-then 1
-when (bore = 15 and type = 'bb' and launched = 1915 and country='USA')
-then 1
-end as mycase
+case when numGuns = 8 then 1 else 0 end as mycase1,
+case when bore = 15 then 1 else 0 end as mycase2,
+case when displacement = 32000 then 1 else 0 end as mycase3,
+case when type = 'bb' then 1 else 0 end as mycase4,
+case when launched = 1915 then 1 else 0 end as mycase5,
+case when a.class='Kongo' then 1 else 0 end as mycase6,
+case when country='USA' then 1 else 0 end as mycase7 
 from ships a
 left join classes b on a.class=b.class
 )
 select name
 from v0
-where mycase=1</t>
+where (mycase1+mycase2+mycase3+mycase4+mycase5+mycase6+mycase7)&gt;3</t>
+  </si>
+  <si>
+    <t>Найти производителей, которые выпускают только принтеры или только PC.
+При этом искомые производители PC должны выпускать не менее 3 моделей.</t>
+  </si>
+  <si>
+    <t>with v0 as (
+Select coalesce(maker, maker) as maker, coalesce(type, type) as types
+from product
+group by coalesce(maker, maker), coalesce(type, type)
+)
+select maker, GROUP_CONCAT (types) types
+from v0
+group by maker
+order by type</t>
+  </si>
+  <si>
+    <t>Для каждого производителя перечислить в алфавитном порядке с разделителем "/" все типы выпускаемой им продукции.
+Вывод: maker, список типов продукции</t>
+  </si>
+  <si>
+    <t>WITH v0 AS (
+  -- взять уникальные комбинации мейкер и тайп
+  SELECT DISTINCT
+    maker,
+    type
+  FROM Product
+),v1 AS (
+  -- вывести тех кто производит только 1 тип
+  SELECT
+    maker,
+    MIN(type) AS min
+  FROM v0
+  GROUP BY maker
+  HAVING COUNT(1) = 1
+)
+-- производители принтера
+SELECT DISTINCT
+  maker
+FROM Product
+WHERE type = 'Printer'
+  AND maker IN (
+  SELECT
+    maker
+  FROM v1
+)
+UNION
+-- производители пк
+SELECT
+  maker
+FROM Product
+WHERE type = 'PC'
+  AND maker IN (
+  SELECT
+    maker
+  FROM v1
+)
+GROUP BY maker
+HAVING COUNT(1) &gt; 2</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +2016,24 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2306,11 +2356,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,7 +3515,7 @@
       </c>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>83</v>
       </c>
@@ -3475,39 +3525,68 @@
       <c r="C80" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E80" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F80" s="12"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="E80" s="5"/>
+      <c r="F80" s="11"/>
+    </row>
+    <row r="81" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>85</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E81" s="5"/>
+      <c r="F81" s="11"/>
+    </row>
+    <row r="82" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>86</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E82" s="5"/>
+      <c r="F82" s="14"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C83" s="6"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="14"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="1:6" ht="405" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" ht="405" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
         <v>56</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B85" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C82" s="16" t="s">
+      <c r="C85" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="F82" s="14" t="s">
+      <c r="F85" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C86" s="2"/>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="2"/>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C89" s="2"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G82"/>
+  <autoFilter ref="A1:G85"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
89, 90 were added
</commit_message>
<xml_diff>
--- a/Задания по SQL.xlsx
+++ b/Задания по SQL.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$G$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$G$86</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="226">
   <si>
     <t>Запрос:</t>
   </si>
@@ -1382,37 +1382,6 @@
     <t>В PyCharm</t>
   </si>
   <si>
-    <t xml:space="preserve">  -- вывести список классов кораблей которые участвовали в битвах с четным числом
--- outcomes(ship,battle), battles(name,date)
--- /2==0
-WITH potential_ships AS (
-  SELECT
-    name,
-    class
-  FROM Ships
-  UNION
-  SELECT
-    class,
-    class
-  FROM Classes
-)
-SELECT
-  class,
-  SUM(
-    CASE WHEN b.date % 2 = 0 THEN 1
-         ELSE 0 END
-    )
-FROM potential_ships p
-  LEFT JOIN Outcomes o
-    ON o.ship = p.name
-  LEFT JOIN Battles b
-    ON b.name = o.battle
-GROUP BY class;</t>
-  </si>
-  <si>
-    <t>Было написано в 56-ом дополнительно</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -1462,9 +1431,6 @@
 where year&lt;&gt;launched
 group by name
 </t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>WITH potential_ships AS (
@@ -1630,20 +1596,6 @@
 select name
 from Ships
 where name=class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select maker, a.model, price, d.type
-from PC a
-right join product d on a.model=d.model
-union 
-select maker, b.model, price, d.type
-from laptop b
-right join product d on b.model=d.model
-union 
-select maker, c.model, price, d.type
-from printer c
-right join product d on c.model=d.model
-</t>
   </si>
   <si>
     <t>Для тех производителей, у которых есть продукты с известной ценой хотя бы в одной из таблиц Laptop, PC, Printer найти максимальные цены на каждый из типов продукции.
@@ -1868,6 +1820,75 @@
 )
 GROUP BY maker
 HAVING COUNT(1) &gt; 2</t>
+  </si>
+  <si>
+    <t>WITH v0 AS (
+  SELECT
+    maker,
+    a.model,
+    price,
+    d.type
+  FROM PC a RIGHT JOIN product d
+  ON a.model=d.model
+  UNION
+  SELECT
+    maker, b.model, price, d.type
+  FROM laptop b
+    RIGHT JOIN product d
+  ON b.model=d.model
+  UNION
+  SELECT
+    maker, c.model, price, d.type
+  FROM printer c
+    RIGHT JOIN product d
+  ON c.model=d.model
+)
+SELECT
+  maker,
+  CASE WHEN (type = 'Laptop') THEN MAX(price) END AS laptop,
+  CASE WHEN (type = 'PC') THEN MAX(price) END AS pc,
+  CASE WHEN (type = 'Printer') THEN MAX(price) END AS printer
+FROM v0
+where price is not NULL
+GROUP BY MAKER, TYPE</t>
+  </si>
+  <si>
+    <t>Найти производителей, у которых больше всего моделей в таблице Product, а также тех, у которых меньше всего моделей.
+Вывод: maker, число моделей</t>
+  </si>
+  <si>
+    <t>Вывести все строки из таблицы Product, кроме трех строк с наименьшими номерами моделей и трех строк с наибольшими номерами моделей.</t>
+  </si>
+  <si>
+    <t>select *
+from product
+where model not in (
+select top 3 model
+from product
+order by model DESC)
+AND
+model not in (
+select top 3 model
+from product
+order by model)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WITH v0 AS (
+  SELECT
+    maker,
+    COUNT(model) AS qty
+  FROM Product
+  GROUP BY maker
+)
+SELECT
+  a.maker, a.qty
+  FROM v0 a, v0 b, v0 c
+GROUP BY a.maker, a.qty
+HAVING MIN(b.qty)=a.qty or MAX(c.qty)=a.qty
+</t>
+  </si>
+  <si>
+    <t>не вносила</t>
   </si>
 </sst>
 </file>
@@ -1916,7 +1937,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1947,6 +1968,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1960,7 +1993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2012,24 +2045,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2356,11 +2387,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,7 +2431,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2407,7 +2439,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2415,7 +2447,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2423,7 +2455,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2431,7 +2463,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2439,7 +2471,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2447,7 +2479,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2455,7 +2487,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2463,7 +2495,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2471,7 +2503,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2485,7 +2517,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2501,7 +2533,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2517,7 +2549,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2533,7 +2565,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2549,7 +2581,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2565,7 +2597,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2581,7 +2613,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2597,7 +2629,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2613,7 +2645,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2629,7 +2661,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2645,8 +2677,8 @@
       <c r="E21" s="1"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2661,7 +2693,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2677,7 +2709,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:6" ht="270" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2693,7 +2725,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2709,7 +2741,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:6" ht="270" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2727,7 +2759,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2735,17 +2767,17 @@
         <v>138</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2761,7 +2793,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2777,7 +2809,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2793,7 +2825,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2809,7 +2841,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2822,7 +2854,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2837,7 +2869,7 @@
       </c>
       <c r="F33" s="15"/>
     </row>
-    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2853,7 +2885,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2869,7 +2901,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2885,7 +2917,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="78.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2893,17 +2925,17 @@
         <v>52</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2919,7 +2951,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2933,8 +2965,9 @@
         <v>55</v>
       </c>
       <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:8" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2952,7 +2985,7 @@
       </c>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2960,21 +2993,21 @@
         <v>144</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="223.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2992,7 +3025,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3008,7 +3041,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="11"/>
     </row>
-    <row r="44" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3016,17 +3049,17 @@
         <v>76</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3040,11 +3073,11 @@
         <v>89</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F45" s="12"/>
     </row>
-    <row r="46" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3060,7 +3093,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="11"/>
     </row>
-    <row r="47" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3078,25 +3111,25 @@
       </c>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>84</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F48" s="11"/>
     </row>
-    <row r="49" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3112,7 +3145,7 @@
       <c r="E49" s="1"/>
       <c r="F49" s="11"/>
     </row>
-    <row r="50" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3128,7 +3161,7 @@
       <c r="E50" s="1"/>
       <c r="F50" s="11"/>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -3144,7 +3177,7 @@
       <c r="E51" s="1"/>
       <c r="F51" s="11"/>
     </row>
-    <row r="52" spans="1:6" s="9" customFormat="1" ht="405" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="9" customFormat="1" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -3159,7 +3192,7 @@
       </c>
       <c r="F52" s="13"/>
     </row>
-    <row r="53" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3170,11 +3203,11 @@
         <v>101</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3188,11 +3221,11 @@
         <v>104</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F54" s="12"/>
     </row>
-    <row r="55" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3206,11 +3239,11 @@
         <v>106</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F55" s="12"/>
     </row>
-    <row r="56" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3226,7 +3259,7 @@
       <c r="E56" s="1"/>
       <c r="F56" s="11"/>
     </row>
-    <row r="57" spans="1:6" ht="270" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3239,7 +3272,7 @@
       <c r="E57" s="1"/>
       <c r="F57" s="11"/>
     </row>
-    <row r="58" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3247,14 +3280,14 @@
         <v>112</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F58" s="12"/>
     </row>
-    <row r="59" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>58</v>
       </c>
@@ -3265,11 +3298,11 @@
         <v>124</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F59" s="11"/>
     </row>
-    <row r="60" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3297,21 +3330,21 @@
       <c r="E61" s="1"/>
       <c r="F61" s="14"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="C62" s="6"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="C63" s="6"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3322,11 +3355,11 @@
         <v>117</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3339,38 +3372,38 @@
       <c r="E65" s="1"/>
       <c r="F65" s="11"/>
     </row>
-    <row r="66" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="11"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3386,7 +3419,7 @@
       <c r="E70" s="1"/>
       <c r="F70" s="11"/>
     </row>
-    <row r="71" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3394,12 +3427,12 @@
         <v>119</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="11"/>
     </row>
-    <row r="72" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3417,7 +3450,7 @@
       </c>
       <c r="F72" s="15"/>
     </row>
-    <row r="73" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3432,7 +3465,7 @@
       </c>
       <c r="F73" s="12"/>
     </row>
-    <row r="74" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3448,10 +3481,10 @@
       <c r="E74" s="1"/>
       <c r="F74" s="11"/>
       <c r="H74" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3464,18 +3497,18 @@
       <c r="E75" s="1"/>
       <c r="F75" s="11"/>
     </row>
-    <row r="76" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E76" s="1"/>
     </row>
@@ -3484,10 +3517,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E77" s="1"/>
     </row>
@@ -3496,47 +3529,50 @@
         <v>77</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>120</v>
       </c>
       <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="F78" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F79" s="11"/>
     </row>
-    <row r="80" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>83</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="11"/>
     </row>
-    <row r="81" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>85</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="11"/>
@@ -3546,47 +3582,69 @@
         <v>86</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>221</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="D82" s="20"/>
       <c r="E82" s="5"/>
       <c r="F82" s="14"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C83" s="6"/>
+    <row r="83" spans="1:6" ht="195" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>89</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>224</v>
+      </c>
       <c r="E83" s="5"/>
-      <c r="F83" s="14"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="1:6" ht="405" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>56</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C85" s="16" t="s">
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="1:6" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>90</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E84" s="5"/>
+      <c r="F84" s="12"/>
+    </row>
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="6"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="14"/>
+    </row>
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F85" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C89" s="2"/>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="2"/>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C88" s="2"/>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G85"/>
+  <autoFilter ref="A1:G86">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3607,57 +3665,57 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
         <v>197</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>198</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>199</v>
       </c>
-      <c r="D1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>200</v>
-      </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C2" s="17">
         <v>1915</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G2" s="17">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I2" s="17">
         <v>32000</v>
@@ -3665,17 +3723,17 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -3688,7 +3746,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -3702,7 +3760,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -3718,7 +3776,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C12" s="18"/>
       <c r="G12" s="18"/>
@@ -3734,7 +3792,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D13" s="18"/>
       <c r="G13" s="18"/>
@@ -3750,7 +3808,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E14" s="18"/>
       <c r="H14" s="18"/>
@@ -3762,7 +3820,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F15" s="18"/>
       <c r="I15" s="18"/>

</xml_diff>